<commit_message>
frontend test case add to report
</commit_message>
<xml_diff>
--- a/Docs/test case.xlsx
+++ b/Docs/test case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IPAuTSoNS\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{310A44C7-6544-413D-BB4A-71075BC473F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5DE29E-4B38-4951-B5AF-F6EC8088C748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{991F98D8-83ED-40C7-89F6-E547C833F51B}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{991F98D8-83ED-40C7-89F6-E547C833F51B}"/>
   </bookViews>
   <sheets>
     <sheet name="frontend" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="209">
   <si>
     <t>Test case - Frontend</t>
   </si>
@@ -313,6 +313,357 @@
   </si>
   <si>
     <t xml:space="preserve">Drive page call api backend and get display data correctly </t>
+  </si>
+  <si>
+    <t>Drive page can display all image folder that user owned</t>
+  </si>
+  <si>
+    <t>Drive page can sent new image folder data to api backend</t>
+  </si>
+  <si>
+    <t>Drive page can sent delete image folder data to api backend</t>
+  </si>
+  <si>
+    <t>Drive page can download chosen image folder in zip file format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drive page can enter chosen image folder </t>
+  </si>
+  <si>
+    <t>Image folder page can authenticate image folder owner user</t>
+  </si>
+  <si>
+    <t>Image folder page can show pop up window to alert when user that authenticate is not image folder owner user</t>
+  </si>
+  <si>
+    <t>Image folder page can sent upload images data to backend by press upload button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image folder page can sent delete image to api backend by press delete button on image </t>
+  </si>
+  <si>
+    <t>Image folder page can make web browser download image data from api backend by press download button on image</t>
+  </si>
+  <si>
+    <t>Image folder page can select range of image to display by select options image folder page</t>
+  </si>
+  <si>
+    <t>Image folder page can show full quality image by press on image card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marketplace page can call api backend and get display data correctly </t>
+  </si>
+  <si>
+    <t>Marketplace page can display products data correctly</t>
+  </si>
+  <si>
+    <t>Marketplace page can go to to Add product page by press add product button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marketplace page can change display products order to lastest product update first </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marketplace page can change display products order to oldest product update first </t>
+  </si>
+  <si>
+    <t>F-054</t>
+  </si>
+  <si>
+    <t>Marketplace page can change display products order to specific date only</t>
+  </si>
+  <si>
+    <t>F-055</t>
+  </si>
+  <si>
+    <t>Marketplace page can change display products type filter</t>
+  </si>
+  <si>
+    <t>F-056</t>
+  </si>
+  <si>
+    <t>Marketplace page can change display products model filter</t>
+  </si>
+  <si>
+    <t>F-057</t>
+  </si>
+  <si>
+    <t>F-058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product page can call api backend and get display data correctly  </t>
+  </si>
+  <si>
+    <t>F-059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product page can display product data correctly  </t>
+  </si>
+  <si>
+    <t>F-060</t>
+  </si>
+  <si>
+    <t>Product page can show pop up window to alert when product is not exited and redirection to Marketplace page</t>
+  </si>
+  <si>
+    <t>F-061</t>
+  </si>
+  <si>
+    <t>F-062</t>
+  </si>
+  <si>
+    <t>F-063</t>
+  </si>
+  <si>
+    <t>F-064</t>
+  </si>
+  <si>
+    <t>F-065</t>
+  </si>
+  <si>
+    <t>F-066</t>
+  </si>
+  <si>
+    <t>F-067</t>
+  </si>
+  <si>
+    <t>F-068</t>
+  </si>
+  <si>
+    <t>F-069</t>
+  </si>
+  <si>
+    <t>F-070</t>
+  </si>
+  <si>
+    <t>F-071</t>
+  </si>
+  <si>
+    <t>F-072</t>
+  </si>
+  <si>
+    <t>F-073</t>
+  </si>
+  <si>
+    <t>F-074</t>
+  </si>
+  <si>
+    <t>F-075</t>
+  </si>
+  <si>
+    <t>F-076</t>
+  </si>
+  <si>
+    <t>F-077</t>
+  </si>
+  <si>
+    <t>F-078</t>
+  </si>
+  <si>
+    <t>Product page can show edit this product button and view product use history button when user is authenticate as product owner</t>
+  </si>
+  <si>
+    <t>Product page can add product to open product list by press try this product button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User setting page can call api backend and get display data correctly  </t>
+  </si>
+  <si>
+    <t>User setting page can display user data correctly</t>
+  </si>
+  <si>
+    <t>User setting page can be change only firstname and lastname of user data</t>
+  </si>
+  <si>
+    <t>User setting page can sent changed user data to api bcakend when press submit button</t>
+  </si>
+  <si>
+    <t>User setting page can show pop up window to alert when change is not compelete</t>
+  </si>
+  <si>
+    <t>User setting page can show pop up window to alert when change is compelete</t>
+  </si>
+  <si>
+    <t>User setting page can go to Change password page when press change password button</t>
+  </si>
+  <si>
+    <t>Change password page display user data correctly</t>
+  </si>
+  <si>
+    <t>Change password page can check password and password confirm is match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change password page can send user old pasword and new password to api backend when press </t>
+  </si>
+  <si>
+    <t>User setting page can clear value in all input form by press clear button</t>
+  </si>
+  <si>
+    <t>Change password page can show pop up window to alert when change is not compelete</t>
+  </si>
+  <si>
+    <t>Change password page can show pop up window to alert when change is compelete</t>
+  </si>
+  <si>
+    <t>Change password page can clear value in all input form by press clear button</t>
+  </si>
+  <si>
+    <t>User setting page all form must be filled when press submit button</t>
+  </si>
+  <si>
+    <t>Change password page all form must be filled when press submit button</t>
+  </si>
+  <si>
+    <t>F-079</t>
+  </si>
+  <si>
+    <t>F-080</t>
+  </si>
+  <si>
+    <t>F-081</t>
+  </si>
+  <si>
+    <t>F-082</t>
+  </si>
+  <si>
+    <t>F-083</t>
+  </si>
+  <si>
+    <t>F-084</t>
+  </si>
+  <si>
+    <t>F-085</t>
+  </si>
+  <si>
+    <t>F-086</t>
+  </si>
+  <si>
+    <t>F-087</t>
+  </si>
+  <si>
+    <t>Marketplace page can go to Product page by press on product card</t>
+  </si>
+  <si>
+    <t>Add product page can call api backend</t>
+  </si>
+  <si>
+    <t>Add product page user can filled all form</t>
+  </si>
+  <si>
+    <t>Add product page user can upload product weight file when press chosse product weight file upload button</t>
+  </si>
+  <si>
+    <t>Add product page user can upload product image when press chosse product image upload button</t>
+  </si>
+  <si>
+    <t>Add product page can check all form are filled when press add product button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add product page can show pop up window to alert when add product process is success </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add product page can show pop up window to alert when add product process is unsuccess </t>
+  </si>
+  <si>
+    <t>Edit product data page user can filled all form</t>
+  </si>
+  <si>
+    <t>Edit product data page user can upload product image when press chosse product image upload button</t>
+  </si>
+  <si>
+    <t>Edit product data page user can upload product weight file when press chosse product weight file upload button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit product data page can show pop up window to alert when edit product data process is success </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit product data page can show pop up window to alert when edit product data process is unsuccess </t>
+  </si>
+  <si>
+    <t>Edit product data page can call api backend and display product data correctly</t>
+  </si>
+  <si>
+    <t>F-088</t>
+  </si>
+  <si>
+    <t>F-089</t>
+  </si>
+  <si>
+    <t>F-090</t>
+  </si>
+  <si>
+    <t>F-091</t>
+  </si>
+  <si>
+    <t>F-092</t>
+  </si>
+  <si>
+    <t>F-093</t>
+  </si>
+  <si>
+    <t>F-094</t>
+  </si>
+  <si>
+    <t>F-095</t>
+  </si>
+  <si>
+    <t>F-096</t>
+  </si>
+  <si>
+    <t>F-097</t>
+  </si>
+  <si>
+    <t>F-098</t>
+  </si>
+  <si>
+    <t>F-099</t>
+  </si>
+  <si>
+    <t>F-100</t>
+  </si>
+  <si>
+    <t>Image processing application page can call api backend and get display data correctly</t>
+  </si>
+  <si>
+    <t>Image processing application page can display all image folders of user correctly</t>
+  </si>
+  <si>
+    <t>Image processing application page can display all product that user opened correctly</t>
+  </si>
+  <si>
+    <t>Image processing application page can display user chosen image from list of all images from chosen image folder when press image thumbnail</t>
+  </si>
+  <si>
+    <t>Image processing application page can display list of all images from user chosen image folder when select image folder in image folder list</t>
+  </si>
+  <si>
+    <t>Image processing application page user can select product to preview product processing result with chosen image</t>
+  </si>
+  <si>
+    <t>Image processing application page user can change parameter of preview product processing result with chosen image</t>
+  </si>
+  <si>
+    <t>Image processing application page can display result image of preview product processing result</t>
+  </si>
+  <si>
+    <t>Image processing application page user can sent order job to api backend when press export button</t>
+  </si>
+  <si>
+    <t>F-101</t>
+  </si>
+  <si>
+    <t>F-102</t>
+  </si>
+  <si>
+    <t>F-103</t>
+  </si>
+  <si>
+    <t>Image processing application page can pop up window to alert when credit payment is require</t>
+  </si>
+  <si>
+    <t>Image processing application page can pop up window to alert when job is on processing</t>
+  </si>
+  <si>
+    <t>Image processing application page can pop up window to alert when job is fail to processing</t>
   </si>
 </sst>
 </file>
@@ -384,14 +735,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
@@ -706,422 +1058,856 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F9C0DE-023F-4407-BD87-02CFE00C37E5}">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B105" sqref="A2:B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="96.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="112.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="3"/>
+      <c r="B39" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="3"/>
+      <c r="B40" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="3"/>
+      <c r="B41" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="3"/>
+      <c r="B42" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="3"/>
+      <c r="B43" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="3"/>
+      <c r="B44" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="3"/>
+      <c r="B45" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="3"/>
+      <c r="B46" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="3"/>
+      <c r="B47" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="3"/>
+      <c r="B48" s="4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="3"/>
+      <c r="B49" s="4" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="3"/>
+      <c r="B50" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B51" s="3"/>
+      <c r="B51" s="4" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="3"/>
+      <c r="B52" s="4" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B53" s="3"/>
+      <c r="B53" s="4" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B54" s="3"/>
+      <c r="B54" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B55" s="3"/>
+      <c r="B55" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>208</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add backend test case to report
</commit_message>
<xml_diff>
--- a/Docs/test case.xlsx
+++ b/Docs/test case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IPAuTSoNS\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5DE29E-4B38-4951-B5AF-F6EC8088C748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8601C7-6CEE-42CD-AF3F-775A3AF3AEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{991F98D8-83ED-40C7-89F6-E547C833F51B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{991F98D8-83ED-40C7-89F6-E547C833F51B}"/>
   </bookViews>
   <sheets>
     <sheet name="frontend" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="312">
   <si>
     <t>Test case - Frontend</t>
   </si>
@@ -664,6 +664,315 @@
   </si>
   <si>
     <t>Image processing application page can pop up window to alert when job is fail to processing</t>
+  </si>
+  <si>
+    <t>B-001</t>
+  </si>
+  <si>
+    <t>B-002</t>
+  </si>
+  <si>
+    <t>B-003</t>
+  </si>
+  <si>
+    <t>B-004</t>
+  </si>
+  <si>
+    <t>B-005</t>
+  </si>
+  <si>
+    <t>B-006</t>
+  </si>
+  <si>
+    <t>B-007</t>
+  </si>
+  <si>
+    <t>B-008</t>
+  </si>
+  <si>
+    <t>B-009</t>
+  </si>
+  <si>
+    <t>B-010</t>
+  </si>
+  <si>
+    <t>B-011</t>
+  </si>
+  <si>
+    <t>B-012</t>
+  </si>
+  <si>
+    <t>B-013</t>
+  </si>
+  <si>
+    <t>B-014</t>
+  </si>
+  <si>
+    <t>B-015</t>
+  </si>
+  <si>
+    <t>B-016</t>
+  </si>
+  <si>
+    <t>B-017</t>
+  </si>
+  <si>
+    <t>B-018</t>
+  </si>
+  <si>
+    <t>B-019</t>
+  </si>
+  <si>
+    <t>B-020</t>
+  </si>
+  <si>
+    <t>B-021</t>
+  </si>
+  <si>
+    <t>B-022</t>
+  </si>
+  <si>
+    <t>B-023</t>
+  </si>
+  <si>
+    <t>B-024</t>
+  </si>
+  <si>
+    <t>B-025</t>
+  </si>
+  <si>
+    <t>B-026</t>
+  </si>
+  <si>
+    <t>B-027</t>
+  </si>
+  <si>
+    <t>B-028</t>
+  </si>
+  <si>
+    <t>B-029</t>
+  </si>
+  <si>
+    <t>B-030</t>
+  </si>
+  <si>
+    <t>B-031</t>
+  </si>
+  <si>
+    <t>B-032</t>
+  </si>
+  <si>
+    <t>B-033</t>
+  </si>
+  <si>
+    <t>B-034</t>
+  </si>
+  <si>
+    <t>B-035</t>
+  </si>
+  <si>
+    <t>B-036</t>
+  </si>
+  <si>
+    <t>B-037</t>
+  </si>
+  <si>
+    <t>B-038</t>
+  </si>
+  <si>
+    <t>B-039</t>
+  </si>
+  <si>
+    <t>B-040</t>
+  </si>
+  <si>
+    <t>B-041</t>
+  </si>
+  <si>
+    <t>B-042</t>
+  </si>
+  <si>
+    <t>B-043</t>
+  </si>
+  <si>
+    <t>B-044</t>
+  </si>
+  <si>
+    <t>B-045</t>
+  </si>
+  <si>
+    <t>B-046</t>
+  </si>
+  <si>
+    <t>B-047</t>
+  </si>
+  <si>
+    <t>B-048</t>
+  </si>
+  <si>
+    <t>B-049</t>
+  </si>
+  <si>
+    <t>B-050</t>
+  </si>
+  <si>
+    <t>B-051</t>
+  </si>
+  <si>
+    <t>Test case - Backend</t>
+  </si>
+  <si>
+    <t>Backend can start and using at configuration IP address</t>
+  </si>
+  <si>
+    <t>Backend can display backend develop version at url /api/ for checking version</t>
+  </si>
+  <si>
+    <t>Backend must authenticate user token in any method when have call from frontend</t>
+  </si>
+  <si>
+    <t>Backend can send response message back to frontend if able to regis new user</t>
+  </si>
+  <si>
+    <t>Backend can send response error message back to frontend if unable to regis new user</t>
+  </si>
+  <si>
+    <t>Backend can send response error message back to frontend if unable to login</t>
+  </si>
+  <si>
+    <t>Backend can make and send response with user authenticate token and user data back to frontend if able to login</t>
+  </si>
+  <si>
+    <t>Backend can send response message back to frontend if able to edit user data</t>
+  </si>
+  <si>
+    <t>Backend can send response error message back to frontend if unable to edit user data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can edit user data in database </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can add new user data to database </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can edit user password in database </t>
+  </si>
+  <si>
+    <t>Backend can send response message back to frontend if able to edit user password</t>
+  </si>
+  <si>
+    <t>Backend can send response error message back to frontend if unable to edit user password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can add user login log to database </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response massage with user job order history qurry to frontend </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response massage with user credit earn and pay history qurry to frontend </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response massage with user image folders qurry to frontend </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response massage with compress image data in selected image folder to frontend </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response massage with full size image data of selected image to frontend </t>
+  </si>
+  <si>
+    <t>Backend can send response massage to frontend if able to add new image folder</t>
+  </si>
+  <si>
+    <t>Backend can add new image folder data to database and create folder in NAS</t>
+  </si>
+  <si>
+    <t>Backend can recive image datas and image files to add to database and store in NAS</t>
+  </si>
+  <si>
+    <t>Backend can send response error massage to frontend if unable to add new image folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response error massage to frontend if unable to add new image </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response massage to frontend if able to add new image </t>
+  </si>
+  <si>
+    <t>Backend can add delete image folder data to database and delete folder in NAS</t>
+  </si>
+  <si>
+    <t>Backend can send response massage to frontend if able to delete image folder</t>
+  </si>
+  <si>
+    <t>Backend can send response error massage to frontend if unable to delete image folder</t>
+  </si>
+  <si>
+    <t>Backend can delete image data from database and delete image from NAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response massage to frontend if able to delete new image </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response error massage to frontend if unable to delete new image </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response massage to frontend if able to download new image </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response error massage to frontend if unable to download new image </t>
+  </si>
+  <si>
+    <t>Backend can send response massage with product list qurry to frontend</t>
+  </si>
+  <si>
+    <t>Backend can send response massage with product data to frontend</t>
+  </si>
+  <si>
+    <t>Backend can send response error massage to frontend if unable to qurry product list</t>
+  </si>
+  <si>
+    <t>Backend can send response error massage to frontend if unable to find product</t>
+  </si>
+  <si>
+    <t>Backend can recive product image file ,weight file and product data to add to database and store in NAS</t>
+  </si>
+  <si>
+    <t>Backend can recive product image file ,weight file and product data to edit product data database and store in NAS</t>
+  </si>
+  <si>
+    <t>Backend can send response massage to frontend if able to edit product data</t>
+  </si>
+  <si>
+    <t>Backend can send response error massage to frontend if unable to edit product data</t>
+  </si>
+  <si>
+    <t>Backend can send response massage to frontend if able to add new product data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend can send response error massage to frontend if unable to add new product data </t>
+  </si>
+  <si>
+    <t>Backend can recive open product data to add to database</t>
+  </si>
+  <si>
+    <t>Backend can recive image data and product data for send to API preview and get result image</t>
+  </si>
+  <si>
+    <t>Backend can send preview result image to frontend</t>
+  </si>
+  <si>
+    <t>Backend can recive product data, parameter and image folder for order image processing job</t>
+  </si>
+  <si>
+    <t>Backend can send response massage to frontend if able to order image processing job</t>
+  </si>
+  <si>
+    <t>Backend can send response error massage to frontend if unable to order image processing job</t>
+  </si>
+  <si>
+    <t>Backend can send response massage with credit payment require to frontend</t>
   </si>
 </sst>
 </file>
@@ -735,15 +1044,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
@@ -1060,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F9C0DE-023F-4407-BD87-02CFE00C37E5}">
   <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B105" sqref="A2:B105"/>
+    <sheetView topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4"/>
@@ -1072,773 +1382,773 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="2" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="2" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="2" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="2" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:2">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="2" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="2" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="2" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="2" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="2" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:2">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="2" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="2" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="2" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="2" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="2" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="2" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="2" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="93" spans="1:2">
-      <c r="A93" s="4" t="s">
+      <c r="A93" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="2" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="4" t="s">
+      <c r="A94" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="2" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" s="4" t="s">
+      <c r="A95" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="2" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="2" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -1846,7 +2156,7 @@
       </c>
     </row>
     <row r="98" spans="1:2">
-      <c r="A98" s="4" t="s">
+      <c r="A98" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B98" s="2" t="s">
@@ -1854,7 +2164,7 @@
       </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="4" t="s">
+      <c r="A99" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B99" s="2" t="s">
@@ -1862,7 +2172,7 @@
       </c>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" s="4" t="s">
+      <c r="A100" s="2" t="s">
         <v>191</v>
       </c>
       <c r="B100" s="2" t="s">
@@ -1870,7 +2180,7 @@
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -1878,7 +2188,7 @@
       </c>
     </row>
     <row r="102" spans="1:2">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="2" t="s">
         <v>193</v>
       </c>
       <c r="B102" s="2" t="s">
@@ -1886,7 +2196,7 @@
       </c>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B103" s="2" t="s">
@@ -1894,7 +2204,7 @@
       </c>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B104" s="2" t="s">
@@ -1902,7 +2212,7 @@
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="2" t="s">
         <v>205</v>
       </c>
       <c r="B105" s="2" t="s">
@@ -1921,14 +2231,702 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723A3704-BBC0-4DDF-A54B-E0048ED86DF0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="116.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.4">
+      <c r="A1" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" ht="23.4">
+      <c r="A2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="23.4">
+      <c r="A3" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="23.4">
+      <c r="A4" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="23.4">
+      <c r="A5" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="23.4">
+      <c r="A6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23.4">
+      <c r="A7" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23.4">
+      <c r="A8" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="23.4">
+      <c r="A9" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="23.4">
+      <c r="A10" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="23.4">
+      <c r="A11" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="23.4">
+      <c r="A12" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="23.4">
+      <c r="A13" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="23.4">
+      <c r="A14" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="23.4">
+      <c r="A15" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="23.4">
+      <c r="A16" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23.4">
+      <c r="A17" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="23.4">
+      <c r="A18" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="23.4">
+      <c r="A19" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="23.4">
+      <c r="A20" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="23.4">
+      <c r="A21" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="23.4">
+      <c r="A22" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="23.4">
+      <c r="A23" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="23.4">
+      <c r="A24" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="23.4">
+      <c r="A25" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="23.4">
+      <c r="A26" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="23.4">
+      <c r="A27" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="23.4">
+      <c r="A28" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="23.4">
+      <c r="A29" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="23.4">
+      <c r="A30" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="23.4">
+      <c r="A31" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="23.4">
+      <c r="A32" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="23.4">
+      <c r="A33" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="23.4">
+      <c r="A34" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="23.4">
+      <c r="A35" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="23.4">
+      <c r="A36" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="23.4">
+      <c r="A37" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="23.4">
+      <c r="A38" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="23.4">
+      <c r="A39" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="23.4">
+      <c r="A40" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="23.4">
+      <c r="A41" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="23.4">
+      <c r="A42" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="23.4">
+      <c r="A43" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="23.4">
+      <c r="A44" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="23.4">
+      <c r="A45" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="23.4">
+      <c r="A46" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="23.4">
+      <c r="A47" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="23.4">
+      <c r="A48" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="23.4">
+      <c r="A49" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="23.4">
+      <c r="A50" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="23.4">
+      <c r="A51" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="23.4">
+      <c r="A52" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="23.4">
+      <c r="A53" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="23.4">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+    </row>
+    <row r="55" spans="1:2" ht="23.4">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+    </row>
+    <row r="56" spans="1:2" ht="23.4">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+    </row>
+    <row r="57" spans="1:2" ht="23.4">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+    </row>
+    <row r="58" spans="1:2" ht="23.4">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" spans="1:2" ht="23.4">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+    </row>
+    <row r="60" spans="1:2" ht="23.4">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+    </row>
+    <row r="61" spans="1:2" ht="23.4">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+    </row>
+    <row r="62" spans="1:2" ht="23.4">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+    </row>
+    <row r="63" spans="1:2" ht="23.4">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+    </row>
+    <row r="64" spans="1:2" ht="23.4">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+    </row>
+    <row r="65" spans="1:2" ht="23.4">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+    </row>
+    <row r="66" spans="1:2" ht="23.4">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+    </row>
+    <row r="67" spans="1:2" ht="23.4">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+    </row>
+    <row r="68" spans="1:2" ht="23.4">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+    </row>
+    <row r="69" spans="1:2" ht="23.4">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+    </row>
+    <row r="70" spans="1:2" ht="23.4">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+    </row>
+    <row r="71" spans="1:2" ht="23.4">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+    </row>
+    <row r="72" spans="1:2" ht="23.4">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+    </row>
+    <row r="73" spans="1:2" ht="23.4">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+    </row>
+    <row r="74" spans="1:2" ht="23.4">
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+    </row>
+    <row r="75" spans="1:2" ht="23.4">
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
+    </row>
+    <row r="76" spans="1:2" ht="23.4">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+    </row>
+    <row r="77" spans="1:2" ht="23.4">
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+    </row>
+    <row r="78" spans="1:2" ht="23.4">
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
+    </row>
+    <row r="79" spans="1:2" ht="23.4">
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
+    </row>
+    <row r="80" spans="1:2" ht="23.4">
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+    </row>
+    <row r="81" spans="1:2" ht="23.4">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
+    </row>
+    <row r="82" spans="1:2" ht="23.4">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+    </row>
+    <row r="83" spans="1:2" ht="23.4">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+    </row>
+    <row r="84" spans="1:2" ht="23.4">
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
+    </row>
+    <row r="85" spans="1:2" ht="23.4">
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+    </row>
+    <row r="86" spans="1:2" ht="23.4">
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
+    </row>
+    <row r="87" spans="1:2" ht="23.4">
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
+    </row>
+    <row r="88" spans="1:2" ht="23.4">
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
+    </row>
+    <row r="89" spans="1:2" ht="23.4">
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
+    </row>
+    <row r="90" spans="1:2" ht="23.4">
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
+    </row>
+    <row r="91" spans="1:2" ht="23.4">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+    </row>
+    <row r="92" spans="1:2" ht="23.4">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
+    </row>
+    <row r="93" spans="1:2" ht="23.4">
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+    </row>
+    <row r="94" spans="1:2" ht="23.4">
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
+    </row>
+    <row r="95" spans="1:2" ht="23.4">
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
+    </row>
+    <row r="96" spans="1:2" ht="23.4">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+    </row>
+    <row r="97" spans="1:2" ht="23.4">
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
+    </row>
+    <row r="98" spans="1:2" ht="23.4">
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
+    </row>
+    <row r="99" spans="1:2" ht="23.4">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
+    </row>
+    <row r="100" spans="1:2" ht="23.4">
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
+    </row>
+    <row r="101" spans="1:2" ht="23.4">
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
+    </row>
+    <row r="102" spans="1:2" ht="23.4">
+      <c r="A102" s="5"/>
+      <c r="B102" s="5"/>
+    </row>
+    <row r="103" spans="1:2" ht="23.4">
+      <c r="A103" s="5"/>
+      <c r="B103" s="5"/>
+    </row>
+    <row r="104" spans="1:2" ht="23.4">
+      <c r="A104" s="5"/>
+      <c r="B104" s="5"/>
+    </row>
+    <row r="105" spans="1:2" ht="23.4">
+      <c r="A105" s="5"/>
+      <c r="B105" s="5"/>
+    </row>
+    <row r="106" spans="1:2" ht="23.4">
+      <c r="A106" s="5"/>
+      <c r="B106" s="5"/>
+    </row>
+    <row r="107" spans="1:2" ht="23.4">
+      <c r="B107" s="1"/>
+    </row>
+    <row r="108" spans="1:2" ht="23.4">
+      <c r="B108" s="1"/>
+    </row>
+    <row r="109" spans="1:2" ht="23.4">
+      <c r="B109" s="1"/>
+    </row>
+    <row r="110" spans="1:2" ht="23.4">
+      <c r="B110" s="1"/>
+    </row>
+    <row r="111" spans="1:2" ht="23.4">
+      <c r="B111" s="1"/>
+    </row>
+    <row r="112" spans="1:2" ht="23.4">
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" spans="2:2" ht="23.4">
+      <c r="B113" s="1"/>
+    </row>
+    <row r="114" spans="2:2" ht="23.4">
+      <c r="B114" s="1"/>
+    </row>
+    <row r="115" spans="2:2" ht="23.4">
+      <c r="B115" s="1"/>
+    </row>
+    <row r="116" spans="2:2" ht="23.4">
+      <c r="B116" s="1"/>
+    </row>
+    <row r="117" spans="2:2" ht="23.4">
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="2:2" ht="23.4">
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="2:2" ht="23.4">
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="2:2" ht="23.4">
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="2:2" ht="23.4">
+      <c r="B121" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>